<commit_message>
updat  mappings rmove duplicate value type
</commit_message>
<xml_diff>
--- a/Log-FHIR.xlsx
+++ b/Log-FHIR.xlsx
@@ -13,17 +13,17 @@
   </sheets>
   <definedNames>
     <definedName name="ActivityDefinition" localSheetId="0">Sheet1!$C$19</definedName>
-    <definedName name="ActivityDefinition.description" localSheetId="0">Sheet1!$C$71</definedName>
-    <definedName name="ActivityDefinition.experimental" localSheetId="0">Sheet1!$C$64</definedName>
+    <definedName name="ActivityDefinition.description" localSheetId="0">Sheet1!$C$70</definedName>
+    <definedName name="ActivityDefinition.experimental" localSheetId="0">Sheet1!$C$63</definedName>
     <definedName name="ActivityDefinition.identifier" localSheetId="0">Sheet1!$C$28</definedName>
-    <definedName name="ActivityDefinition.lastReviewDate" localSheetId="0">Sheet1!$C$89</definedName>
+    <definedName name="ActivityDefinition.lastReviewDate" localSheetId="0">Sheet1!$C$88</definedName>
     <definedName name="ActivityDefinition.name" localSheetId="0">Sheet1!$C$44</definedName>
-    <definedName name="ActivityDefinition.publicationDate" localSheetId="0">Sheet1!$C$85</definedName>
-    <definedName name="ActivityDefinition.purpose" localSheetId="0">Sheet1!$C$76</definedName>
-    <definedName name="ActivityDefinition.status" localSheetId="0">Sheet1!$C$56</definedName>
-    <definedName name="ActivityDefinition.title" localSheetId="0">Sheet1!$C$51</definedName>
+    <definedName name="ActivityDefinition.publicationDate" localSheetId="0">Sheet1!$C$84</definedName>
+    <definedName name="ActivityDefinition.purpose" localSheetId="0">Sheet1!$C$75</definedName>
+    <definedName name="ActivityDefinition.status" localSheetId="0">Sheet1!$C$55</definedName>
+    <definedName name="ActivityDefinition.title" localSheetId="0">Sheet1!$C$50</definedName>
     <definedName name="ActivityDefinition.url" localSheetId="0">Sheet1!$C$22</definedName>
-    <definedName name="ActivityDefinition.usage" localSheetId="0">Sheet1!$C$81</definedName>
+    <definedName name="ActivityDefinition.usage" localSheetId="0">Sheet1!$C$80</definedName>
     <definedName name="ActivityDefinition.version" localSheetId="0">Sheet1!$C$36</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -168,9 +168,6 @@
     <t>LabTestCatalog.entry.measurement.Critical</t>
   </si>
   <si>
-    <t>LabTestCatalog.entry.measurement.valueType</t>
-  </si>
-  <si>
     <t>LabTestCatalog.entry.measurement.units</t>
   </si>
   <si>
@@ -520,6 +517,9 @@
   </si>
   <si>
     <t>referenceRange.text</t>
+  </si>
+  <si>
+    <t>Observation.referenceRange.meaning = "critical"</t>
   </si>
 </sst>
 </file>
@@ -859,13 +859,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H90"/>
+  <dimension ref="A1:H89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B35" sqref="B35"/>
+      <selection pane="bottomRight" activeCell="A47" sqref="A47:XFD47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -881,25 +881,25 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" t="s">
         <v>89</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>90</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>91</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>93</v>
       </c>
-      <c r="F1" t="s">
-        <v>94</v>
-      </c>
       <c r="G1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H1" t="str">
         <f>A1&amp;"--&gt;"&amp;B1&amp;"."&amp;C1&amp;" {"&amp;D1&amp;"|"&amp;E1&amp;"} Rule: "&amp;F1&amp;".  (EH 9/2016 Comment: "&amp;G1&amp;")"</f>
@@ -911,19 +911,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H2" t="str">
-        <f t="shared" ref="H2:H65" si="0">A2&amp;"--&gt;"&amp;B2&amp;"."&amp;C2&amp;" {"&amp;D2&amp;"|"&amp;E2&amp;"} Rule: "&amp;F2&amp;".  (EH 9/2016 Comment: "&amp;G2&amp;")"</f>
+        <f t="shared" ref="H2:H64" si="0">A2&amp;"--&gt;"&amp;B2&amp;"."&amp;C2&amp;" {"&amp;D2&amp;"|"&amp;E2&amp;"} Rule: "&amp;F2&amp;".  (EH 9/2016 Comment: "&amp;G2&amp;")"</f>
         <v>LabTestCatalog--&gt;Bundle.root {|} Rule: .type = "collection".  (EH 9/2016 Comment: Also consider Document for publishing or ActivityDefinition here as well ( could bundle contain link to a pdf?))</v>
       </c>
     </row>
@@ -932,10 +932,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" si="0"/>
@@ -947,10 +947,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
@@ -962,13 +962,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" si="0"/>
@@ -980,13 +980,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="0"/>
@@ -998,13 +998,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" si="0"/>
@@ -1016,13 +1016,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" si="0"/>
@@ -1034,13 +1034,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C9" t="s">
+        <v>100</v>
+      </c>
+      <c r="G9" t="s">
         <v>101</v>
-      </c>
-      <c r="G9" t="s">
-        <v>102</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" si="0"/>
@@ -1052,13 +1052,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10" t="s">
         <v>103</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G10" t="s">
-        <v>104</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="0"/>
@@ -1070,10 +1070,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="0"/>
@@ -1085,13 +1085,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="0"/>
@@ -1103,13 +1103,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
@@ -1121,10 +1121,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
@@ -1136,10 +1136,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="0"/>
@@ -1151,10 +1151,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="0"/>
@@ -1166,10 +1166,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="0"/>
@@ -1181,10 +1181,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="0"/>
@@ -1196,10 +1196,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
@@ -1211,13 +1211,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="0"/>
@@ -1229,13 +1229,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C21" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G21" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="0"/>
@@ -1247,13 +1247,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="0"/>
@@ -1265,10 +1265,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="0"/>
@@ -1280,10 +1280,10 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C24" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
@@ -1295,10 +1295,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="0"/>
@@ -1310,10 +1310,10 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C26" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="0"/>
@@ -1325,13 +1325,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="0"/>
@@ -1343,10 +1343,10 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="0"/>
@@ -1358,10 +1358,10 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
@@ -1373,10 +1373,10 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
@@ -1388,10 +1388,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
@@ -1403,10 +1403,10 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H32" t="str">
         <f t="shared" si="0"/>
@@ -1418,10 +1418,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="0"/>
@@ -1433,10 +1433,10 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C34" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H34" t="str">
         <f t="shared" si="0"/>
@@ -1448,10 +1448,10 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H35" t="str">
         <f t="shared" si="0"/>
@@ -1463,10 +1463,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="0"/>
@@ -1478,16 +1478,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C37" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F37" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G37" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="0"/>
@@ -1499,13 +1499,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C38" t="s">
+        <v>128</v>
+      </c>
+      <c r="G38" t="s">
         <v>129</v>
-      </c>
-      <c r="G38" t="s">
-        <v>130</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="0"/>
@@ -1517,13 +1517,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C39" t="s">
+        <v>130</v>
+      </c>
+      <c r="G39" t="s">
         <v>131</v>
-      </c>
-      <c r="G39" t="s">
-        <v>132</v>
       </c>
       <c r="H39" t="str">
         <f t="shared" si="0"/>
@@ -1535,10 +1535,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C40" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="0"/>
@@ -1550,10 +1550,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C41" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="0"/>
@@ -1565,13 +1565,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C42" t="s">
+        <v>132</v>
+      </c>
+      <c r="G42" t="s">
         <v>133</v>
-      </c>
-      <c r="G42" t="s">
-        <v>134</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="0"/>
@@ -1583,13 +1583,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
+        <v>134</v>
+      </c>
+      <c r="C43" t="s">
+        <v>160</v>
+      </c>
+      <c r="G43" t="s">
         <v>135</v>
-      </c>
-      <c r="C43" t="s">
-        <v>161</v>
-      </c>
-      <c r="G43" t="s">
-        <v>136</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="0"/>
@@ -1601,16 +1601,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G44" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="0"/>
@@ -1622,16 +1622,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F45" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G45" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="0"/>
@@ -1643,11 +1643,17 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>120</v>
+        <v>119</v>
+      </c>
+      <c r="C46" t="s">
+        <v>161</v>
+      </c>
+      <c r="F46" t="s">
+        <v>162</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.measurement.Critical--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.measurement.Critical--&gt;Observation.referenceRange.text {|} Rule: Observation.referenceRange.meaning = "critical".  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1655,11 +1661,11 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.measurement.valueType--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.measurement.units--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1667,11 +1673,11 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H48" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.measurement.units--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.measurement.UCUM--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1679,11 +1685,11 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.measurement.UCUM--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.measurement.conversion--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1691,11 +1697,11 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H50" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.measurement.conversion--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.measurement.precision--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1703,11 +1709,11 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H51" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.measurement.precision--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.measurement.referenceRange--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1715,11 +1721,11 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H52" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.measurement.referenceRange--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.measurement.criticalReferenceRange--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1727,11 +1733,11 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H53" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.measurement.criticalReferenceRange--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.measurement.absoluteReferenceRange--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1739,11 +1745,11 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="H54" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.measurement.absoluteReferenceRange--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.measurement.performingLab--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1751,11 +1757,14 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>120</v>
+        <v>102</v>
+      </c>
+      <c r="C55" t="s">
+        <v>140</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.measurement.performingLab--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.supportingInformation--&gt;ActivityDefinition..relatedResources type=composed-of Reference(Questionnaire) 0..* {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -1763,14 +1772,11 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>103</v>
-      </c>
-      <c r="C56" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="H56" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.supportingInformation--&gt;ActivityDefinition..relatedResources type=composed-of Reference(Questionnaire) 0..* {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.supportingInformation.code--&gt;Questionnaire. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1778,11 +1784,11 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H57" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.supportingInformation.code--&gt;Questionnaire. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.supportingInformation.whenAsk--&gt;Questionnaire. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -1790,11 +1796,11 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H58" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.supportingInformation.whenAsk--&gt;Questionnaire. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.supportingInformation.required--&gt;Questionnaire. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1802,11 +1808,11 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H59" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.supportingInformation.required--&gt;Questionnaire. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.supportingInformation.hint--&gt;Questionnaire. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -1814,11 +1820,11 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H60" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.supportingInformation.hint--&gt;Questionnaire. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.supportingInformation.answerType--&gt;Questionnaire. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -1826,11 +1832,11 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H61" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.supportingInformation.answerType--&gt;Questionnaire. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.supportingInformation.multiples--&gt;Questionnaire. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -1838,11 +1844,11 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H62" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.supportingInformation.multiples--&gt;Questionnaire. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.supportingInformation.answerList--&gt;Questionnaire. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -1850,11 +1856,11 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H63" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.supportingInformation.answerList--&gt;Questionnaire. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.supportingInformation.length--&gt;Questionnaire. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -1862,11 +1868,11 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H64" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.supportingInformation.length--&gt;Questionnaire. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.supportingInformation.precision--&gt;Questionnaire. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -1874,11 +1880,14 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>121</v>
+        <v>102</v>
+      </c>
+      <c r="C65" t="s">
+        <v>139</v>
       </c>
       <c r="H65" t="str">
-        <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.supportingInformation.precision--&gt;Questionnaire. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <f t="shared" ref="H65:H89" si="1">A65&amp;"--&gt;"&amp;B65&amp;"."&amp;C65&amp;" {"&amp;D65&amp;"|"&amp;E65&amp;"} Rule: "&amp;F65&amp;".  (EH 9/2016 Comment: "&amp;G65&amp;")"</f>
+        <v>LabTestCatalog.entry.specimen--&gt;ActivityDefinition..relatedResources type=composed-of Reference(Specimen) 0..* {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -1886,14 +1895,11 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>103</v>
-      </c>
-      <c r="C66" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="H66" t="str">
-        <f t="shared" ref="H66:H90" si="1">A66&amp;"--&gt;"&amp;B66&amp;"."&amp;C66&amp;" {"&amp;D66&amp;"|"&amp;E66&amp;"} Rule: "&amp;F66&amp;".  (EH 9/2016 Comment: "&amp;G66&amp;")"</f>
-        <v>LabTestCatalog.entry.specimen--&gt;ActivityDefinition..relatedResources type=composed-of Reference(Specimen) 0..* {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <f t="shared" si="1"/>
+        <v>LabTestCatalog.entry.specimen.type--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -1901,11 +1907,11 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H67" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.specimen.type--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.specimen.container--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -1913,11 +1919,11 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H68" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.specimen.container--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.specimen.container.type--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -1925,11 +1931,11 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H69" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.specimen.container.type--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.specimen.container.volume--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -1937,11 +1943,11 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H70" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.specimen.container.volume--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.specimen.container.preferrence--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -1949,11 +1955,11 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H71" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.specimen.container.preferrence--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.specimen.additve--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -1961,11 +1967,11 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H72" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.specimen.additve--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.specimen.collectionVolume--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -1973,11 +1979,11 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H73" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.specimen.collectionVolume--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.specimen.minimumCollectionVolume--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -1985,11 +1991,11 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H74" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.specimen.minimumCollectionVolume--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.specimen.requirements--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -1997,11 +2003,11 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H75" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.specimen.requirements--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.specimen.handling--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2009,11 +2015,11 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H76" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.specimen.handling--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.specimen.preference--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2021,11 +2027,14 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>122</v>
+        <v>102</v>
+      </c>
+      <c r="C77" t="s">
+        <v>141</v>
       </c>
       <c r="H77" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.specimen.preference--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.chargeCharacteristic--&gt;ActivityDefinition..relatedResources type=composed-of Reference(??) 0..* {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2033,14 +2042,11 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>103</v>
-      </c>
-      <c r="C78" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="H78" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.chargeCharacteristic--&gt;ActivityDefinition..relatedResources type=composed-of Reference(??) 0..* {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.chargeCharacteristic.shortName--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2048,11 +2054,11 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H79" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.chargeCharacteristic.shortName--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.chargeCharacteristic.longName--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2060,11 +2066,11 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H80" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.chargeCharacteristic.longName--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.chargeCharacteristic.code--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2072,11 +2078,11 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H81" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.chargeCharacteristic.code--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.chargeCharacteristic.price--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2084,11 +2090,11 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H82" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.chargeCharacteristic.price--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.payerPolicy--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2096,11 +2102,14 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>123</v>
+        <v>102</v>
+      </c>
+      <c r="C83" t="s">
+        <v>141</v>
       </c>
       <c r="H83" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.payerPolicy--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.payerPolicy.healthPlan--&gt;ActivityDefinition..relatedResources type=composed-of Reference(??) 0..* {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2108,14 +2117,11 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>103</v>
-      </c>
-      <c r="C84" t="s">
-        <v>142</v>
+        <v>122</v>
       </c>
       <c r="H84" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.payerPolicy.healthPlan--&gt;ActivityDefinition..relatedResources type=composed-of Reference(??) 0..* {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.payerPolicy.InsCompany--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2123,11 +2129,11 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H85" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.payerPolicy.InsCompany--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.payerPolicy.priceRange--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2135,11 +2141,11 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H86" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.payerPolicy.priceRange--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.payerPolicy.reason--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2147,11 +2153,11 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H87" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.payerPolicy.reason--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.payerPolicy.approvedProcedures--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2159,11 +2165,11 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H88" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.payerPolicy.approvedProcedures--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.payerPolicy.approvedProcedures.dxCode--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2171,21 +2177,9 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="H89" t="str">
-        <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.payerPolicy.approvedProcedures.dxCode--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8">
-      <c r="A90" t="s">
-        <v>88</v>
-      </c>
-      <c r="B90" t="s">
-        <v>123</v>
-      </c>
-      <c r="H90" t="str">
         <f t="shared" si="1"/>
         <v>LabTestCatalog.entry.payerPolicy.approvedProcedures.pxCode--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>

</xml_diff>

<commit_message>
updaet to fhir mappings
</commit_message>
<xml_diff>
--- a/Log-FHIR.xlsx
+++ b/Log-FHIR.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="175">
   <si>
     <t>LabTestCatalog</t>
   </si>
@@ -423,9 +423,6 @@
     <t>extension.valueReference.display,  asume only used in  reports not obs</t>
   </si>
   <si>
-    <t>extension</t>
-  </si>
-  <si>
     <t>This is more like a composition concept instead of DR - discuss</t>
   </si>
   <si>
@@ -520,6 +517,45 @@
   </si>
   <si>
     <t>Observation.referenceRange.meaning = "critical"</t>
+  </si>
+  <si>
+    <t>valueQuantity.unit</t>
+  </si>
+  <si>
+    <t>valuetype = valueQuantity et al</t>
+  </si>
+  <si>
+    <t>valueQuantity.code</t>
+  </si>
+  <si>
+    <t>http://unitsofmeasure.org</t>
+  </si>
+  <si>
+    <t>extension type Integer 0..1</t>
+  </si>
+  <si>
+    <t>extension type string</t>
+  </si>
+  <si>
+    <t>.valueQuantity.value</t>
+  </si>
+  <si>
+    <t>invarient with regex mask</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for other numeric resulted value types as well </t>
+  </si>
+  <si>
+    <t xml:space="preserve">could also be an operation, for other numeric resulted value types as well </t>
+  </si>
+  <si>
+    <t>.referenceRange</t>
+  </si>
+  <si>
+    <t>Observation.referenceRange.meaning = "absolute"</t>
+  </si>
+  <si>
+    <t>.performer.Reference(Organization)</t>
   </si>
 </sst>
 </file>
@@ -862,10 +898,10 @@
   <dimension ref="A1:H89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A47" sqref="A47:XFD47"/>
+      <selection pane="bottomRight" activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -935,7 +971,7 @@
         <v>116</v>
       </c>
       <c r="C3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" si="0"/>
@@ -950,7 +986,7 @@
         <v>116</v>
       </c>
       <c r="C4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
@@ -965,7 +1001,7 @@
         <v>116</v>
       </c>
       <c r="C5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G5" t="s">
         <v>97</v>
@@ -983,7 +1019,7 @@
         <v>116</v>
       </c>
       <c r="C6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G6" t="s">
         <v>97</v>
@@ -1001,7 +1037,7 @@
         <v>116</v>
       </c>
       <c r="C7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G7" t="s">
         <v>97</v>
@@ -1088,7 +1124,7 @@
         <v>123</v>
       </c>
       <c r="C12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G12" t="s">
         <v>106</v>
@@ -1106,7 +1142,7 @@
         <v>102</v>
       </c>
       <c r="C13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G13" t="s">
         <v>124</v>
@@ -1124,7 +1160,7 @@
         <v>102</v>
       </c>
       <c r="C14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
@@ -1199,7 +1235,7 @@
         <v>102</v>
       </c>
       <c r="C19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
@@ -1283,7 +1319,7 @@
         <v>102</v>
       </c>
       <c r="C24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
@@ -1361,7 +1397,7 @@
         <v>102</v>
       </c>
       <c r="C29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
@@ -1376,7 +1412,7 @@
         <v>117</v>
       </c>
       <c r="C30" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
@@ -1391,7 +1427,7 @@
         <v>117</v>
       </c>
       <c r="C31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
@@ -1421,7 +1457,7 @@
         <v>102</v>
       </c>
       <c r="C33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="0"/>
@@ -1466,7 +1502,7 @@
         <v>102</v>
       </c>
       <c r="C36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="0"/>
@@ -1481,7 +1517,7 @@
         <v>127</v>
       </c>
       <c r="C37" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F37" t="s">
         <v>126</v>
@@ -1520,14 +1556,14 @@
         <v>118</v>
       </c>
       <c r="C39" t="s">
+        <v>166</v>
+      </c>
+      <c r="G39" t="s">
         <v>130</v>
       </c>
-      <c r="G39" t="s">
-        <v>131</v>
-      </c>
       <c r="H39" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.report.displayOrder--&gt;DiagnosticReport.extension {|} Rule: .  (EH 9/2016 Comment: This is more like a composition concept instead of DR - discuss)</v>
+        <v>LabTestCatalog.entry.report.displayOrder--&gt;DiagnosticReport.extension type Integer 0..1 {|} Rule: .  (EH 9/2016 Comment: This is more like a composition concept instead of DR - discuss)</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1538,7 +1574,7 @@
         <v>102</v>
       </c>
       <c r="C40" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="0"/>
@@ -1553,7 +1589,7 @@
         <v>119</v>
       </c>
       <c r="C41" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="0"/>
@@ -1568,10 +1604,10 @@
         <v>119</v>
       </c>
       <c r="C42" t="s">
+        <v>131</v>
+      </c>
+      <c r="G42" t="s">
         <v>132</v>
-      </c>
-      <c r="G42" t="s">
-        <v>133</v>
       </c>
       <c r="H42" t="str">
         <f t="shared" si="0"/>
@@ -1583,13 +1619,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
+        <v>133</v>
+      </c>
+      <c r="C43" t="s">
+        <v>159</v>
+      </c>
+      <c r="G43" t="s">
         <v>134</v>
-      </c>
-      <c r="C43" t="s">
-        <v>160</v>
-      </c>
-      <c r="G43" t="s">
-        <v>135</v>
       </c>
       <c r="H43" t="str">
         <f t="shared" si="0"/>
@@ -1604,13 +1640,13 @@
         <v>119</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F44" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H44" t="str">
         <f t="shared" si="0"/>
@@ -1625,13 +1661,13 @@
         <v>119</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F45" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G45" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H45" t="str">
         <f t="shared" si="0"/>
@@ -1646,10 +1682,10 @@
         <v>119</v>
       </c>
       <c r="C46" t="s">
+        <v>160</v>
+      </c>
+      <c r="F46" t="s">
         <v>161</v>
-      </c>
-      <c r="F46" t="s">
-        <v>162</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="0"/>
@@ -1663,9 +1699,18 @@
       <c r="B47" t="s">
         <v>119</v>
       </c>
+      <c r="C47" t="s">
+        <v>162</v>
+      </c>
+      <c r="F47" t="s">
+        <v>163</v>
+      </c>
+      <c r="G47" t="s">
+        <v>170</v>
+      </c>
       <c r="H47" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.measurement.units--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.measurement.units--&gt;Observation.valueQuantity.unit {|} Rule: valuetype = valueQuantity et al.  (EH 9/2016 Comment: for other numeric resulted value types as well )</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1675,9 +1720,18 @@
       <c r="B48" t="s">
         <v>119</v>
       </c>
+      <c r="C48" t="s">
+        <v>164</v>
+      </c>
+      <c r="E48" t="s">
+        <v>165</v>
+      </c>
+      <c r="G48" t="s">
+        <v>170</v>
+      </c>
       <c r="H48" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.measurement.UCUM--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.measurement.UCUM--&gt;Observation.valueQuantity.code {|http://unitsofmeasure.org} Rule: .  (EH 9/2016 Comment: for other numeric resulted value types as well )</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1687,9 +1741,15 @@
       <c r="B49" t="s">
         <v>119</v>
       </c>
+      <c r="C49" t="s">
+        <v>167</v>
+      </c>
+      <c r="G49" t="s">
+        <v>171</v>
+      </c>
       <c r="H49" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.measurement.conversion--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.measurement.conversion--&gt;Observation.extension type string {|} Rule: .  (EH 9/2016 Comment: could also be an operation, for other numeric resulted value types as well )</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1699,9 +1759,18 @@
       <c r="B50" t="s">
         <v>119</v>
       </c>
+      <c r="C50" t="s">
+        <v>168</v>
+      </c>
+      <c r="F50" t="s">
+        <v>169</v>
+      </c>
+      <c r="G50" t="s">
+        <v>170</v>
+      </c>
       <c r="H50" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.measurement.precision--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.measurement.precision--&gt;Observation..valueQuantity.value {|} Rule: invarient with regex mask.  (EH 9/2016 Comment: for other numeric resulted value types as well )</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1711,9 +1780,15 @@
       <c r="B51" t="s">
         <v>119</v>
       </c>
+      <c r="C51" t="s">
+        <v>172</v>
+      </c>
+      <c r="F51" t="s">
+        <v>136</v>
+      </c>
       <c r="H51" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.measurement.referenceRange--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.measurement.referenceRange--&gt;Observation..referenceRange {|} Rule: Observation.referenceRange.meaning = "normal".  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1723,9 +1798,15 @@
       <c r="B52" t="s">
         <v>119</v>
       </c>
+      <c r="C52" t="s">
+        <v>172</v>
+      </c>
+      <c r="F52" t="s">
+        <v>161</v>
+      </c>
       <c r="H52" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.measurement.criticalReferenceRange--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.measurement.criticalReferenceRange--&gt;Observation..referenceRange {|} Rule: Observation.referenceRange.meaning = "critical".  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1735,9 +1816,15 @@
       <c r="B53" t="s">
         <v>119</v>
       </c>
+      <c r="C53" t="s">
+        <v>172</v>
+      </c>
+      <c r="F53" t="s">
+        <v>173</v>
+      </c>
       <c r="H53" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.measurement.absoluteReferenceRange--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.measurement.absoluteReferenceRange--&gt;Observation..referenceRange {|} Rule: Observation.referenceRange.meaning = "absolute".  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1747,9 +1834,12 @@
       <c r="B54" t="s">
         <v>119</v>
       </c>
+      <c r="C54" t="s">
+        <v>174</v>
+      </c>
       <c r="H54" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.measurement.performingLab--&gt;Observation. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.measurement.performingLab--&gt;Observation..performer.Reference(Organization) {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1760,7 +1850,7 @@
         <v>102</v>
       </c>
       <c r="C55" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="0"/>
@@ -1883,7 +1973,7 @@
         <v>102</v>
       </c>
       <c r="C65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H65" t="str">
         <f t="shared" ref="H65:H89" si="1">A65&amp;"--&gt;"&amp;B65&amp;"."&amp;C65&amp;" {"&amp;D65&amp;"|"&amp;E65&amp;"} Rule: "&amp;F65&amp;".  (EH 9/2016 Comment: "&amp;G65&amp;")"</f>
@@ -2030,7 +2120,7 @@
         <v>102</v>
       </c>
       <c r="C77" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H77" t="str">
         <f t="shared" si="1"/>
@@ -2105,7 +2195,7 @@
         <v>102</v>
       </c>
       <c r="C83" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H83" t="str">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
finished draft of fhir mappings
</commit_message>
<xml_diff>
--- a/Log-FHIR.xlsx
+++ b/Log-FHIR.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="205">
   <si>
     <t>LabTestCatalog</t>
   </si>
@@ -414,9 +414,6 @@
     <t>Specimen</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>ActivityDefinition|DiagnosticRequest|DiagnosticReport|Observation</t>
   </si>
   <si>
@@ -438,6 +435,9 @@
     <t>extension.valueReference.display,  asume only used in  reports not obs</t>
   </si>
   <si>
+    <t>extension</t>
+  </si>
+  <si>
     <t>This is more like a composition concept instead of DR - discuss</t>
   </si>
   <si>
@@ -462,15 +462,6 @@
     <t>Observation.referenceRange.meaning = "abnormal"</t>
   </si>
   <si>
-    <t>.relatedResources type=composed-of Reference(Specimen) 0..*</t>
-  </si>
-  <si>
-    <t>.relatedResources type=composed-of Reference(Questionnaire) 0..*</t>
-  </si>
-  <si>
-    <t>.relatedResources type=composed-of Reference(??) 0..*</t>
-  </si>
-  <si>
     <t>meta.extension type=Reference(Organization) 0.1</t>
   </si>
   <si>
@@ -552,9 +543,6 @@
     <t>extension type string</t>
   </si>
   <si>
-    <t>.valueQuantity.value</t>
-  </si>
-  <si>
     <t>invarient with regex mask</t>
   </si>
   <si>
@@ -564,43 +552,115 @@
     <t xml:space="preserve">could also be an operation, for other numeric resulted value types as well </t>
   </si>
   <si>
-    <t>.referenceRange</t>
-  </si>
-  <si>
     <t>Observation.referenceRange.meaning = "absolute"</t>
   </si>
   <si>
-    <t>.performer.Reference(Organization)</t>
-  </si>
-  <si>
-    <t>Questionnaire.useContext</t>
-  </si>
-  <si>
-    <t>Questionnaire.item.concept</t>
-  </si>
-  <si>
     <t>single questionnaire for each provider role each filling in her part</t>
   </si>
   <si>
-    <t>Questionnaire.item.required</t>
-  </si>
-  <si>
-    <t>Questionnaire.item.text</t>
-  </si>
-  <si>
-    <t>Questionnaire.item.type</t>
-  </si>
-  <si>
-    <t>Questionnaire.item.repeats</t>
-  </si>
-  <si>
-    <t>Questionnaire.item.options</t>
-  </si>
-  <si>
-    <t>Questionnaire.item.maxLength</t>
-  </si>
-  <si>
-    <t>Questionnaire.extension(http://hl7.org/fhir/StructureDefinition/maxDecimalPlaces)</t>
+    <t>type</t>
+  </si>
+  <si>
+    <t>container</t>
+  </si>
+  <si>
+    <t>container.type</t>
+  </si>
+  <si>
+    <t>container.capacity</t>
+  </si>
+  <si>
+    <t>container.extension type boolean 0..1</t>
+  </si>
+  <si>
+    <t>add this to the description of the field?</t>
+  </si>
+  <si>
+    <t>have this as an invariant.  (e.g   &gt;=  1.0 ml)</t>
+  </si>
+  <si>
+    <t>extension(ttp://hl7.org/fhir/StructureDefinition/specimen-specialHandling)</t>
+  </si>
+  <si>
+    <t>item.concept</t>
+  </si>
+  <si>
+    <t>useContext</t>
+  </si>
+  <si>
+    <t>item.required</t>
+  </si>
+  <si>
+    <t>item.text</t>
+  </si>
+  <si>
+    <t>item.type</t>
+  </si>
+  <si>
+    <t>item.repeats</t>
+  </si>
+  <si>
+    <t>item.options</t>
+  </si>
+  <si>
+    <t>item.maxLength</t>
+  </si>
+  <si>
+    <t>extension(http://hl7.org/fhir/StructureDefinition/maxDecimalPlaces)</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>collection.quantity</t>
+  </si>
+  <si>
+    <t>treatment.additive or container.additive[x]</t>
+  </si>
+  <si>
+    <t>valueQuantity.value</t>
+  </si>
+  <si>
+    <t>referenceRange</t>
+  </si>
+  <si>
+    <t>performer.Reference(Organization)</t>
+  </si>
+  <si>
+    <t>relatedResources type=composed-of Reference(Questionnaire) 0..*</t>
+  </si>
+  <si>
+    <t>relatedResources type=composed-of Reference(Specimen) 0..*</t>
+  </si>
+  <si>
+    <t>Claim</t>
+  </si>
+  <si>
+    <t>item.unitPrice</t>
+  </si>
+  <si>
+    <t>insurerIdentifier</t>
+  </si>
+  <si>
+    <t>diagnosis.diagnosis</t>
+  </si>
+  <si>
+    <t>procedure.procedure[x]</t>
+  </si>
+  <si>
+    <t>relatedResources type=composed-of Reference(??) 0..*</t>
+  </si>
+  <si>
+    <t>item.service.display</t>
+  </si>
+  <si>
+    <t>item.service.extension type = string 0..1</t>
+  </si>
+  <si>
+    <t>item.service.code</t>
+  </si>
+  <si>
+    <t>coverage.coverageIdentifier</t>
   </si>
 </sst>
 </file>
@@ -943,10 +1003,10 @@
   <dimension ref="A1:H89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C52" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B57" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C66" sqref="C66"/>
+      <selection pane="bottomRight" activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1016,7 +1076,7 @@
         <v>116</v>
       </c>
       <c r="C3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H3" t="str">
         <f t="shared" si="0"/>
@@ -1031,7 +1091,7 @@
         <v>116</v>
       </c>
       <c r="C4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H4" t="str">
         <f t="shared" si="0"/>
@@ -1046,7 +1106,7 @@
         <v>116</v>
       </c>
       <c r="C5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G5" t="s">
         <v>97</v>
@@ -1064,7 +1124,7 @@
         <v>116</v>
       </c>
       <c r="C6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="G6" t="s">
         <v>97</v>
@@ -1082,7 +1142,7 @@
         <v>116</v>
       </c>
       <c r="C7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G7" t="s">
         <v>97</v>
@@ -1166,10 +1226,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C12" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="G12" t="s">
         <v>106</v>
@@ -1187,10 +1247,10 @@
         <v>102</v>
       </c>
       <c r="C13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="0"/>
@@ -1205,7 +1265,7 @@
         <v>102</v>
       </c>
       <c r="C14" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="0"/>
@@ -1280,7 +1340,7 @@
         <v>102</v>
       </c>
       <c r="C19" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="0"/>
@@ -1364,7 +1424,7 @@
         <v>102</v>
       </c>
       <c r="C24" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="0"/>
@@ -1442,7 +1502,7 @@
         <v>102</v>
       </c>
       <c r="C29" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="0"/>
@@ -1457,7 +1517,7 @@
         <v>117</v>
       </c>
       <c r="C30" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="0"/>
@@ -1472,7 +1532,7 @@
         <v>117</v>
       </c>
       <c r="C31" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H31" t="str">
         <f t="shared" si="0"/>
@@ -1502,7 +1562,7 @@
         <v>102</v>
       </c>
       <c r="C33" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H33" t="str">
         <f t="shared" si="0"/>
@@ -1547,7 +1607,7 @@
         <v>102</v>
       </c>
       <c r="C36" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H36" t="str">
         <f t="shared" si="0"/>
@@ -1559,16 +1619,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C37" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F37" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G37" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H37" t="str">
         <f t="shared" si="0"/>
@@ -1583,10 +1643,10 @@
         <v>118</v>
       </c>
       <c r="C38" t="s">
+        <v>127</v>
+      </c>
+      <c r="G38" t="s">
         <v>128</v>
-      </c>
-      <c r="G38" t="s">
-        <v>129</v>
       </c>
       <c r="H38" t="str">
         <f t="shared" si="0"/>
@@ -1601,7 +1661,7 @@
         <v>118</v>
       </c>
       <c r="C39" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G39" t="s">
         <v>130</v>
@@ -1619,7 +1679,7 @@
         <v>102</v>
       </c>
       <c r="C40" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H40" t="str">
         <f t="shared" si="0"/>
@@ -1634,7 +1694,7 @@
         <v>119</v>
       </c>
       <c r="C41" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H41" t="str">
         <f t="shared" si="0"/>
@@ -1667,7 +1727,7 @@
         <v>133</v>
       </c>
       <c r="C43" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="G43" t="s">
         <v>134</v>
@@ -1685,7 +1745,7 @@
         <v>119</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F44" t="s">
         <v>136</v>
@@ -1706,7 +1766,7 @@
         <v>119</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F45" t="s">
         <v>137</v>
@@ -1727,10 +1787,10 @@
         <v>119</v>
       </c>
       <c r="C46" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F46" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H46" t="str">
         <f t="shared" si="0"/>
@@ -1745,13 +1805,13 @@
         <v>119</v>
       </c>
       <c r="C47" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F47" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="G47" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="H47" t="str">
         <f t="shared" si="0"/>
@@ -1766,13 +1826,13 @@
         <v>119</v>
       </c>
       <c r="C48" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E48" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G48" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="H48" t="str">
         <f t="shared" si="0"/>
@@ -1787,10 +1847,10 @@
         <v>119</v>
       </c>
       <c r="C49" t="s">
+        <v>164</v>
+      </c>
+      <c r="G49" t="s">
         <v>167</v>
-      </c>
-      <c r="G49" t="s">
-        <v>171</v>
       </c>
       <c r="H49" t="str">
         <f t="shared" si="0"/>
@@ -1805,17 +1865,17 @@
         <v>119</v>
       </c>
       <c r="C50" t="s">
-        <v>168</v>
+        <v>190</v>
       </c>
       <c r="F50" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G50" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="H50" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.measurement.precision--&gt;Observation..valueQuantity.value {|} Rule: invarient with regex mask.  (EH 9/2016 Comment: for other numeric resulted value types as well )</v>
+        <v>LabTestCatalog.entry.measurement.precision--&gt;Observation.valueQuantity.value {|} Rule: invarient with regex mask.  (EH 9/2016 Comment: for other numeric resulted value types as well )</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1826,14 +1886,14 @@
         <v>119</v>
       </c>
       <c r="C51" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="F51" t="s">
         <v>136</v>
       </c>
       <c r="H51" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.measurement.referenceRange--&gt;Observation..referenceRange {|} Rule: Observation.referenceRange.meaning = "normal".  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.measurement.referenceRange--&gt;Observation.referenceRange {|} Rule: Observation.referenceRange.meaning = "normal".  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1844,14 +1904,14 @@
         <v>119</v>
       </c>
       <c r="C52" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="F52" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H52" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.measurement.criticalReferenceRange--&gt;Observation..referenceRange {|} Rule: Observation.referenceRange.meaning = "critical".  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.measurement.criticalReferenceRange--&gt;Observation.referenceRange {|} Rule: Observation.referenceRange.meaning = "critical".  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1862,14 +1922,14 @@
         <v>119</v>
       </c>
       <c r="C53" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="F53" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H53" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.measurement.absoluteReferenceRange--&gt;Observation..referenceRange {|} Rule: Observation.referenceRange.meaning = "absolute".  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.measurement.absoluteReferenceRange--&gt;Observation.referenceRange {|} Rule: Observation.referenceRange.meaning = "absolute".  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1880,11 +1940,11 @@
         <v>119</v>
       </c>
       <c r="C54" t="s">
-        <v>174</v>
+        <v>192</v>
       </c>
       <c r="H54" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.measurement.performingLab--&gt;Observation..performer.Reference(Organization) {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.measurement.performingLab--&gt;Observation.performer.Reference(Organization) {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1895,11 +1955,11 @@
         <v>102</v>
       </c>
       <c r="C55" t="s">
-        <v>139</v>
+        <v>193</v>
       </c>
       <c r="H55" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.supportingInformation--&gt;ActivityDefinition..relatedResources type=composed-of Reference(Questionnaire) 0..* {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.supportingInformation--&gt;ActivityDefinition.relatedResources type=composed-of Reference(Questionnaire) 0..* {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -1910,11 +1970,11 @@
         <v>120</v>
       </c>
       <c r="C56" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="H56" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.supportingInformation.code--&gt;Questionnaire.Questionnaire.item.concept {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.supportingInformation.code--&gt;Questionnaire.item.concept {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1925,14 +1985,14 @@
         <v>120</v>
       </c>
       <c r="C57" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="F57" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="H57" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.supportingInformation.whenAsk--&gt;Questionnaire.Questionnaire.useContext {|} Rule: single questionnaire for each provider role each filling in her part.  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.supportingInformation.whenAsk--&gt;Questionnaire.useContext {|} Rule: single questionnaire for each provider role each filling in her part.  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -1943,11 +2003,11 @@
         <v>120</v>
       </c>
       <c r="C58" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="H58" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.supportingInformation.required--&gt;Questionnaire.Questionnaire.item.required {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.supportingInformation.required--&gt;Questionnaire.item.required {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1958,11 +2018,11 @@
         <v>120</v>
       </c>
       <c r="C59" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="H59" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.supportingInformation.hint--&gt;Questionnaire.Questionnaire.item.text {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.supportingInformation.hint--&gt;Questionnaire.item.text {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -1973,11 +2033,11 @@
         <v>120</v>
       </c>
       <c r="C60" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H60" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.supportingInformation.answerType--&gt;Questionnaire.Questionnaire.item.type {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.supportingInformation.answerType--&gt;Questionnaire.item.type {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -1988,11 +2048,11 @@
         <v>120</v>
       </c>
       <c r="C61" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="H61" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.supportingInformation.multiples--&gt;Questionnaire.Questionnaire.item.repeats {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.supportingInformation.multiples--&gt;Questionnaire.item.repeats {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -2003,11 +2063,11 @@
         <v>120</v>
       </c>
       <c r="C62" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H62" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.supportingInformation.answerList--&gt;Questionnaire.Questionnaire.item.options {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.supportingInformation.answerList--&gt;Questionnaire.item.options {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2018,11 +2078,11 @@
         <v>120</v>
       </c>
       <c r="C63" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="H63" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.supportingInformation.length--&gt;Questionnaire.Questionnaire.item.maxLength {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.supportingInformation.length--&gt;Questionnaire.item.maxLength {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2033,11 +2093,11 @@
         <v>120</v>
       </c>
       <c r="C64" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H64" t="str">
         <f t="shared" si="0"/>
-        <v>LabTestCatalog.entry.supportingInformation.precision--&gt;Questionnaire.Questionnaire.extension(http://hl7.org/fhir/StructureDefinition/maxDecimalPlaces) {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.supportingInformation.precision--&gt;Questionnaire.extension(http://hl7.org/fhir/StructureDefinition/maxDecimalPlaces) {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2048,11 +2108,11 @@
         <v>102</v>
       </c>
       <c r="C65" t="s">
-        <v>138</v>
+        <v>194</v>
       </c>
       <c r="H65" t="str">
         <f t="shared" ref="H65:H89" si="1">A65&amp;"--&gt;"&amp;B65&amp;"."&amp;C65&amp;" {"&amp;D65&amp;"|"&amp;E65&amp;"} Rule: "&amp;F65&amp;".  (EH 9/2016 Comment: "&amp;G65&amp;")"</f>
-        <v>LabTestCatalog.entry.specimen--&gt;ActivityDefinition..relatedResources type=composed-of Reference(Specimen) 0..* {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.specimen--&gt;ActivityDefinition.relatedResources type=composed-of Reference(Specimen) 0..* {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2062,9 +2122,12 @@
       <c r="B66" t="s">
         <v>121</v>
       </c>
+      <c r="C66" t="s">
+        <v>170</v>
+      </c>
       <c r="H66" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.specimen.type--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.specimen.type--&gt;Specimen.type {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2074,9 +2137,12 @@
       <c r="B67" t="s">
         <v>121</v>
       </c>
+      <c r="C67" t="s">
+        <v>171</v>
+      </c>
       <c r="H67" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.specimen.container--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.specimen.container--&gt;Specimen.container {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2086,9 +2152,12 @@
       <c r="B68" t="s">
         <v>121</v>
       </c>
+      <c r="C68" t="s">
+        <v>172</v>
+      </c>
       <c r="H68" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.specimen.container.type--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.specimen.container.type--&gt;Specimen.container.type {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2098,9 +2167,12 @@
       <c r="B69" t="s">
         <v>121</v>
       </c>
+      <c r="C69" t="s">
+        <v>173</v>
+      </c>
       <c r="H69" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.specimen.container.volume--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.specimen.container.volume--&gt;Specimen.container.capacity {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2110,9 +2182,12 @@
       <c r="B70" t="s">
         <v>121</v>
       </c>
+      <c r="C70" t="s">
+        <v>174</v>
+      </c>
       <c r="H70" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.specimen.container.preferrence--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.specimen.container.preferrence--&gt;Specimen.container.extension type boolean 0..1 {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2122,9 +2197,12 @@
       <c r="B71" t="s">
         <v>121</v>
       </c>
+      <c r="C71" t="s">
+        <v>189</v>
+      </c>
       <c r="H71" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.specimen.additve--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.specimen.additve--&gt;Specimen.treatment.additive or container.additive[x] {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2134,9 +2212,15 @@
       <c r="B72" t="s">
         <v>121</v>
       </c>
+      <c r="C72" t="s">
+        <v>188</v>
+      </c>
+      <c r="G72" t="s">
+        <v>175</v>
+      </c>
       <c r="H72" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.specimen.collectionVolume--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.specimen.collectionVolume--&gt;Specimen.collection.quantity {|} Rule: .  (EH 9/2016 Comment: add this to the description of the field?)</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2146,9 +2230,15 @@
       <c r="B73" t="s">
         <v>121</v>
       </c>
+      <c r="C73" t="s">
+        <v>188</v>
+      </c>
+      <c r="G73" t="s">
+        <v>176</v>
+      </c>
       <c r="H73" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.specimen.minimumCollectionVolume--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.specimen.minimumCollectionVolume--&gt;Specimen.collection.quantity {|} Rule: .  (EH 9/2016 Comment: have this as an invariant.  (e.g   &gt;=  1.0 ml))</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2158,9 +2248,12 @@
       <c r="B74" t="s">
         <v>121</v>
       </c>
+      <c r="C74" t="s">
+        <v>187</v>
+      </c>
       <c r="H74" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.specimen.requirements--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.specimen.requirements--&gt;Specimen.note {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2170,9 +2263,12 @@
       <c r="B75" t="s">
         <v>121</v>
       </c>
+      <c r="C75" t="s">
+        <v>177</v>
+      </c>
       <c r="H75" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.specimen.handling--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.specimen.handling--&gt;Specimen.extension(ttp://hl7.org/fhir/StructureDefinition/specimen-specialHandling) {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2180,11 +2276,14 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>121</v>
+        <v>102</v>
+      </c>
+      <c r="C76" t="s">
+        <v>129</v>
       </c>
       <c r="H76" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.specimen.preference--&gt;Specimen. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.specimen.preference--&gt;ActivityDefinition.extension {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2195,11 +2294,11 @@
         <v>102</v>
       </c>
       <c r="C77" t="s">
-        <v>140</v>
+        <v>200</v>
       </c>
       <c r="H77" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.chargeCharacteristic--&gt;ActivityDefinition..relatedResources type=composed-of Reference(??) 0..* {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.chargeCharacteristic--&gt;ActivityDefinition.relatedResources type=composed-of Reference(??) 0..* {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2207,11 +2306,14 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>122</v>
+        <v>195</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="H78" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.chargeCharacteristic.shortName--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.chargeCharacteristic.shortName--&gt;Claim.item.service.display {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2219,11 +2321,14 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>122</v>
+        <v>195</v>
+      </c>
+      <c r="C79" t="s">
+        <v>202</v>
       </c>
       <c r="H79" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.chargeCharacteristic.longName--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.chargeCharacteristic.longName--&gt;Claim.item.service.extension type = string 0..1 {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2231,11 +2336,14 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>122</v>
+        <v>195</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>203</v>
       </c>
       <c r="H80" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.chargeCharacteristic.code--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.chargeCharacteristic.code--&gt;Claim.item.service.code {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2243,11 +2351,14 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>122</v>
+        <v>195</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="H81" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.chargeCharacteristic.price--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.chargeCharacteristic.price--&gt;Claim.item.unitPrice {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2255,11 +2366,11 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>122</v>
+        <v>195</v>
       </c>
       <c r="H82" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.payerPolicy--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.payerPolicy--&gt;Claim. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2267,14 +2378,14 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>102</v>
-      </c>
-      <c r="C83" t="s">
-        <v>140</v>
+        <v>195</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="H83" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.payerPolicy.healthPlan--&gt;ActivityDefinition..relatedResources type=composed-of Reference(??) 0..* {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.payerPolicy.healthPlan--&gt;Claim.insurerIdentifier {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2282,11 +2393,14 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>122</v>
+        <v>195</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>197</v>
       </c>
       <c r="H84" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.payerPolicy.InsCompany--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.payerPolicy.InsCompany--&gt;Claim.insurerIdentifier {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2294,11 +2408,14 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>122</v>
+        <v>195</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>204</v>
       </c>
       <c r="H85" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.payerPolicy.priceRange--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.payerPolicy.priceRange--&gt;Claim.coverage.coverageIdentifier {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2306,11 +2423,14 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>122</v>
+        <v>195</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>129</v>
       </c>
       <c r="H86" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.payerPolicy.reason--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.payerPolicy.reason--&gt;Claim.extension {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2318,11 +2438,11 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>122</v>
+        <v>195</v>
       </c>
       <c r="H87" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.payerPolicy.approvedProcedures--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.payerPolicy.approvedProcedures--&gt;Claim. {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2330,11 +2450,14 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>122</v>
+        <v>195</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="H88" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.payerPolicy.approvedProcedures.dxCode--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.payerPolicy.approvedProcedures.dxCode--&gt;Claim.diagnosis.diagnosis {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2342,11 +2465,14 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>122</v>
+        <v>195</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>199</v>
       </c>
       <c r="H89" t="str">
         <f t="shared" si="1"/>
-        <v>LabTestCatalog.entry.payerPolicy.approvedProcedures.pxCode--&gt;??. {|} Rule: .  (EH 9/2016 Comment: )</v>
+        <v>LabTestCatalog.entry.payerPolicy.approvedProcedures.pxCode--&gt;Claim.procedure.procedure[x] {|} Rule: .  (EH 9/2016 Comment: )</v>
       </c>
     </row>
   </sheetData>

</xml_diff>